<commit_message>
Updated Readme and code
</commit_message>
<xml_diff>
--- a/Multilevel_statistic/Analysis_Develop_WT/data/Kmean_CovM_SummaryDev.xlsx
+++ b/Multilevel_statistic/Analysis_Develop_WT/data/Kmean_CovM_SummaryDev.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/juiyhuan_iu_edu/Documents/Github_Desktop/SubNetwork_search_multilevel2025/Multilevel_statistic/Analysis_Develop_WT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_514D2FFFC806E94F2746EF07E6012D161186356A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0783CBAC-8203-4B36-AC19-5F6DB2CDE34F}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_514D2FFFC806E94F2746EF07E6012D161186356A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0316758D-F332-4C6F-80DC-10937F0F063E}"/>
   <bookViews>
-    <workbookView xWindow="37920" yWindow="8550" windowWidth="38700" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="3060" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1930,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,7 +2436,7 @@
         <v>0.98441345365053323</v>
       </c>
       <c r="O9">
-        <v>7.9787234042553195</v>
+        <v>7.9787234042553203</v>
       </c>
       <c r="P9">
         <v>32.446808510638299</v>

</xml_diff>